<commit_message>
major update on almost everything
</commit_message>
<xml_diff>
--- a/Rider_Ersterfassung_Muster.xlsx
+++ b/Rider_Ersterfassung_Muster.xlsx
@@ -5,14 +5,16 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Frankfurt" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Offenbach" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Frankfurt!$A$1:$F$420</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Frankfurt!$A$1:$I$7</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Offenbach!$A$1:$I$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Frankfurt!$A$1:$F$420</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="28">
   <si>
     <t xml:space="preserve">rider name</t>
   </si>
@@ -38,10 +40,19 @@
     <t xml:space="preserve">city</t>
   </si>
   <si>
-    <t xml:space="preserve">first_entry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">last_entry</t>
+    <t xml:space="preserve">first entry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">last entry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">current contract first entry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prev contracts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">similar names</t>
   </si>
   <si>
     <t xml:space="preserve">Jane Doe</t>
@@ -306,26 +317,34 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="16.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="13.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -347,19 +366,28 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E2" s="4" t="n">
         <v>43617</v>
@@ -370,16 +398,16 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E3" s="4" t="n">
         <v>43617</v>
@@ -390,16 +418,16 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="E4" s="4" t="n">
         <v>43617</v>
@@ -410,16 +438,16 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E5" s="4" t="n">
         <v>43617</v>
@@ -430,16 +458,16 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E6" s="4" t="n">
         <v>43617</v>
@@ -450,16 +478,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E7" s="4" t="n">
         <v>43617</v>
@@ -882,7 +910,7 @@
     <row r="419" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="420" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:F420"/>
+  <autoFilter ref="A1:I7"/>
   <conditionalFormatting sqref="C3:C337">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"NO DATA"</formula>
@@ -944,19 +972,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="16.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -978,19 +1010,28 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E2" s="4" t="n">
         <v>43617</v>
@@ -1001,16 +1042,16 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E3" s="4" t="n">
         <v>43617</v>
@@ -1021,16 +1062,16 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E4" s="4" t="n">
         <v>43617</v>
@@ -1041,16 +1082,16 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="E5" s="4" t="n">
         <v>43617</v>
@@ -1061,16 +1102,16 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E6" s="4" t="n">
         <v>43617</v>
@@ -1081,16 +1122,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E7" s="4" t="n">
         <v>43617</v>
@@ -1100,6 +1141,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I7"/>
   <conditionalFormatting sqref="C4:C337">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"NO DATA"</formula>
@@ -1147,5 +1189,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>